<commit_message>
vault backup: 2024-10-21 22:19:25
</commit_message>
<xml_diff>
--- a/content/杂物间/游戏/Switch/switch下载榜单.xlsx
+++ b/content/杂物间/游戏/Switch/switch下载榜单.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\Switch游戏下载\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13B8F02-2B08-4E5F-9174-967FF8D5556B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12C7E35-7F2B-41F2-AD6F-7404C4D2FB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,7 +769,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -919,7 +919,7 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F7" t="s">

</xml_diff>

<commit_message>
vault backup: 2024-10-23 12:54:11
</commit_message>
<xml_diff>
--- a/content/杂物间/游戏/Switch/switch下载榜单.xlsx
+++ b/content/杂物间/游戏/Switch/switch下载榜单.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\Switch游戏下载\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\Enterprise\content\杂物间\游戏\Switch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12C7E35-7F2B-41F2-AD6F-7404C4D2FB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B41F83-523A-4F4A-BF54-75704A0CBC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,18 +769,18 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -823,7 +823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -840,7 +840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -863,7 +863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -886,7 +886,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -909,7 +909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -952,7 +952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -975,7 +975,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -998,7 +998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1110,12 +1110,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>103</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="J19" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
vault backup: 2024-10-25 11:56:27
</commit_message>
<xml_diff>
--- a/content/杂物间/游戏/Switch/switch下载榜单.xlsx
+++ b/content/杂物间/游戏/Switch/switch下载榜单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\Enterprise\content\杂物间\游戏\Switch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B41F83-523A-4F4A-BF54-75704A0CBC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A3B1B-B4B6-46E6-A7BD-5D02917E8CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,10 +353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>灵魂旅者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>灵魂旅人（者）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -431,6 +427,10 @@
   </si>
   <si>
     <t>逆转裁判系列（查游玩顺序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜡笔小新 煤炭镇的小白</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,18 +769,18 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="36.75" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +791,7 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -823,7 +823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -840,7 +840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -848,10 +848,10 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
         <v>52</v>
@@ -863,7 +863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -886,7 +886,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -909,7 +909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -940,7 +940,7 @@
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -948,11 +948,9 @@
       <c r="J8" t="s">
         <v>75</v>
       </c>
-      <c r="M8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -975,7 +973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -983,10 +981,10 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -998,12 +996,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
@@ -1012,21 +1010,21 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="M11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -1035,7 +1033,7 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" t="s">
         <v>79</v>
@@ -1044,30 +1042,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J14" t="s">
         <v>71</v>
@@ -1090,42 +1088,45 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>